<commit_message>
the legion awakens (supervisor working with robottas.conf)
</commit_message>
<xml_diff>
--- a/modules/data/logs/accounts.xlsx
+++ b/modules/data/logs/accounts.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B116"/>
+  <dimension ref="A1:B122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1596,6 +1596,66 @@
         <v>73535051</v>
       </c>
     </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>J_Montgomery78@yahoo.com</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>26940137</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Caledoni_C@xs4all.nl</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>79667400</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Aile.B52@gmail.com</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>80613716</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Ma.Chavez70@yahoo.com</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>62538332</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>JaG@hotmail.com</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>42152129</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Alexander-JameHansen@xs4all.nl</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>97408675</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>